<commit_message>
WO Consumer advanced search, 80% completed
</commit_message>
<xml_diff>
--- a/Data Files/Consumer_Data.xlsx
+++ b/Data Files/Consumer_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67E18AD-BB49-4B52-AC7B-44F258FFA57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425B82B9-9E6B-4E33-97E2-B8AB194728D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1643D0D5-C3EF-42B5-B3D0-D0BD3D603EDF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1643D0D5-C3EF-42B5-B3D0-D0BD3D603EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Forename</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Brown</t>
   </si>
   <si>
-    <t>gordonbro@gmail.com</t>
-  </si>
-  <si>
     <t>2 Redwood Drive</t>
   </si>
   <si>
@@ -99,17 +96,92 @@
     <t>Consumer_ID</t>
   </si>
   <si>
-    <t>408091</t>
-  </si>
-  <si>
     <t>ALL</t>
+  </si>
+  <si>
+    <t>gordbro@gmail.com</t>
+  </si>
+  <si>
+    <t>r_Title</t>
+  </si>
+  <si>
+    <t>r_Forenames</t>
+  </si>
+  <si>
+    <t>r_Housename</t>
+  </si>
+  <si>
+    <t>r_Number_and_Street</t>
+  </si>
+  <si>
+    <t>r_Fax</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>r_City</t>
+  </si>
+  <si>
+    <t>r_Town</t>
+  </si>
+  <si>
+    <t>r_Postcode</t>
+  </si>
+  <si>
+    <t>r_Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>r_County</t>
+  </si>
+  <si>
+    <t>Redwood Drive</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>No Record Existing</t>
+  </si>
+  <si>
+    <t>r_Phone_1</t>
+  </si>
+  <si>
+    <t>r_Phone_2</t>
+  </si>
+  <si>
+    <t>r_Full_Name</t>
+  </si>
+  <si>
+    <t>r_Full_Address</t>
+  </si>
+  <si>
+    <t>Mr Gordon Brown</t>
+  </si>
+  <si>
+    <r>
+      <t>Haywards Heath, West Sussex, RH16 4ER </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF555555"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>447772535248</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +196,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF181818"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,10 +238,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E619CB5-8108-478F-9ECC-57C8984FDECA}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,9 +586,17 @@
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" customWidth="1"/>
     <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" customWidth="1"/>
+    <col min="20" max="23" width="14" customWidth="1"/>
+    <col min="24" max="24" width="15" customWidth="1"/>
+    <col min="27" max="27" width="20.42578125" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,46 +637,150 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="N2" s="5">
+        <v>5154205</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updates after validator fixes and other related issues
</commit_message>
<xml_diff>
--- a/Data Files/Consumer_Data.xlsx
+++ b/Data Files/Consumer_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425B82B9-9E6B-4E33-97E2-B8AB194728D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E199030-0D9E-4C17-9F95-F8BB7F5691B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1643D0D5-C3EF-42B5-B3D0-D0BD3D603EDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1643D0D5-C3EF-42B5-B3D0-D0BD3D603EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Forename</t>
   </si>
@@ -136,15 +136,6 @@
   </si>
   <si>
     <t>r_County</t>
-  </si>
-  <si>
-    <t>Redwood Drive</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>No Record Existing</t>
   </si>
   <si>
     <t>r_Phone_1</t>
@@ -564,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E619CB5-8108-478F-9ECC-57C8984FDECA}">
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,19 +658,19 @@
         <v>31</v>
       </c>
       <c r="X1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Y1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Z1" t="s">
         <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AB1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -727,10 +718,10 @@
         <v>19</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -745,7 +736,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
@@ -758,29 +749,12 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
       <c r="AA5" s="2"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AA7" s="2"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AA8" s="2"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AA9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>